<commit_message>
Syncing up chart work.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/NPS2024/DoD_2024_NPS_pt2.xlsx
+++ b/Output/AcqTrends/NPS2024/DoD_2024_NPS_pt2.xlsx
@@ -173,9 +173,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -213,10 +213,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1694,17 +1694,17 @@
         <f>AV13</f>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="2" t="str">
+      <c r="G13" s="1" t="str">
         <f>AV13/AU13-1</f>
       </c>
-      <c r="H13" s="2" t="str">
+      <c r="H13" s="1" t="str">
         <f>AV13/AS13-1</f>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="str">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="str">
         <f>AV13/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="1"/>
       <c r="M13" t="s">
         <v>36</v>
       </c>
@@ -1832,17 +1832,17 @@
         <f>AV14</f>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="2" t="str">
+      <c r="G14" s="1" t="str">
         <f>AV14/AU14-1</f>
       </c>
-      <c r="H14" s="2" t="str">
+      <c r="H14" s="1" t="str">
         <f>AV14/AS14-1</f>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="str">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="str">
         <f>AV14/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="1"/>
       <c r="M14" t="s">
         <v>37</v>
       </c>
@@ -1970,17 +1970,17 @@
         <f>AV15</f>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="2" t="str">
+      <c r="G15" s="1" t="str">
         <f>AV15/AU15-1</f>
       </c>
-      <c r="H15" s="2" t="str">
+      <c r="H15" s="1" t="str">
         <f>AV15/AS15-1</f>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2" t="str">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="str">
         <f>AV15/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="1"/>
       <c r="M15" t="s">
         <v>38</v>
       </c>
@@ -2108,17 +2108,17 @@
         <f>AV16</f>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="2" t="str">
+      <c r="G16" s="1" t="str">
         <f>AV16/AU16-1</f>
       </c>
-      <c r="H16" s="2" t="str">
+      <c r="H16" s="1" t="str">
         <f>AV16/AS16-1</f>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="str">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="str">
         <f>AV16/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="1"/>
       <c r="M16" t="s">
         <v>40</v>
       </c>
@@ -2232,17 +2232,17 @@
         <f>AV17</f>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="2" t="str">
+      <c r="G17" s="1" t="str">
         <f>AV17/AU17-1</f>
       </c>
-      <c r="H17" s="2" t="str">
+      <c r="H17" s="1" t="str">
         <f>AV17/AS17-1</f>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="str">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="str">
         <f>AV17/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="1"/>
       <c r="M17" t="s">
         <v>42</v>
       </c>
@@ -2362,17 +2362,17 @@
         <f>AV18</f>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="2" t="str">
+      <c r="G18" s="1" t="str">
         <f>AV18/AU18-1</f>
       </c>
-      <c r="H18" s="2" t="str">
+      <c r="H18" s="1" t="str">
         <f>AV18/AS18-1</f>
       </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2" t="str">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="str">
         <f>AV18/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="1"/>
       <c r="M18" t="s">
         <v>41</v>
       </c>
@@ -2500,17 +2500,17 @@
         <f>AV19</f>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="2" t="str">
+      <c r="G19" s="1" t="str">
         <f>AV19/AU19-1</f>
       </c>
-      <c r="H19" s="2" t="str">
+      <c r="H19" s="1" t="str">
         <f>AV19/AS19-1</f>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2" t="str">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="str">
         <f>AV19/Sum(AV$12:AV$19)</f>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="1"/>
       <c r="M19" t="s">
         <v>39</v>
       </c>
@@ -2638,17 +2638,17 @@
         <f>AV20</f>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="2" t="str">
+      <c r="G20" s="1" t="str">
         <f>AV20/AU20-1</f>
       </c>
-      <c r="H20" s="2" t="str">
+      <c r="H20" s="1" t="str">
         <f>AV20/AS20-1</f>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="str">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="str">
         <f>Sum(J$12:J$19)</f>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="1"/>
       <c r="M20" t="s">
         <v>43</v>
       </c>
@@ -5372,17 +5372,17 @@
         <f>AV30</f>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="2" t="str">
+      <c r="G30" s="1" t="str">
         <f>AV30/AU30-1</f>
       </c>
-      <c r="H30" s="2" t="str">
+      <c r="H30" s="1" t="str">
         <f>AV30/AS30-1</f>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2" t="str">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1" t="str">
         <f>AV30/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K30" s="2"/>
+      <c r="K30" s="1"/>
       <c r="M30" t="s">
         <v>47</v>
       </c>
@@ -5490,17 +5490,17 @@
         <f>AV31</f>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="2" t="str">
+      <c r="G31" s="1" t="str">
         <f>AV31/AU31-1</f>
       </c>
-      <c r="H31" s="2" t="str">
+      <c r="H31" s="1" t="str">
         <f>AV31/AS31-1</f>
       </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2" t="str">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1" t="str">
         <f>AV31/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K31" s="2"/>
+      <c r="K31" s="1"/>
       <c r="M31" t="s">
         <v>47</v>
       </c>
@@ -5608,17 +5608,17 @@
         <f>AV32</f>
       </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="2" t="str">
+      <c r="G32" s="1" t="str">
         <f>AV32/AU32-1</f>
       </c>
-      <c r="H32" s="2" t="str">
+      <c r="H32" s="1" t="str">
         <f>AV32/AS32-1</f>
       </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2" t="str">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="str">
         <f>AV32/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K32" s="2"/>
+      <c r="K32" s="1"/>
       <c r="M32" t="s">
         <v>47</v>
       </c>
@@ -5726,17 +5726,17 @@
         <f>AV33</f>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="2" t="str">
+      <c r="G33" s="1" t="str">
         <f>AV33/AU33-1</f>
       </c>
-      <c r="H33" s="2" t="str">
+      <c r="H33" s="1" t="str">
         <f>AV33/AS33-1</f>
       </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2" t="str">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="str">
         <f>AV33/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K33" s="2"/>
+      <c r="K33" s="1"/>
       <c r="M33" t="s">
         <v>47</v>
       </c>
@@ -5844,17 +5844,17 @@
         <f>AV34</f>
       </c>
       <c r="F34" s="3"/>
-      <c r="G34" s="2" t="str">
+      <c r="G34" s="1" t="str">
         <f>AV34/AU34-1</f>
       </c>
-      <c r="H34" s="2" t="str">
+      <c r="H34" s="1" t="str">
         <f>AV34/AS34-1</f>
       </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2" t="str">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1" t="str">
         <f>AV34/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K34" s="2"/>
+      <c r="K34" s="1"/>
       <c r="M34" t="s">
         <v>47</v>
       </c>
@@ -5962,17 +5962,17 @@
         <f>AV35</f>
       </c>
       <c r="F35" s="3"/>
-      <c r="G35" s="2" t="str">
+      <c r="G35" s="1" t="str">
         <f>AV35/AU35-1</f>
       </c>
-      <c r="H35" s="2" t="str">
+      <c r="H35" s="1" t="str">
         <f>AV35/AS35-1</f>
       </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2" t="str">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1" t="str">
         <f>AV35/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K35" s="2"/>
+      <c r="K35" s="1"/>
       <c r="M35" t="s">
         <v>47</v>
       </c>
@@ -6080,17 +6080,17 @@
         <f>AV36</f>
       </c>
       <c r="F36" s="3"/>
-      <c r="G36" s="2" t="str">
+      <c r="G36" s="1" t="str">
         <f>AV36/AU36-1</f>
       </c>
-      <c r="H36" s="2" t="str">
+      <c r="H36" s="1" t="str">
         <f>AV36/AS36-1</f>
       </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2" t="str">
+      <c r="I36" s="1"/>
+      <c r="J36" s="1" t="str">
         <f>AV36/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K36" s="2"/>
+      <c r="K36" s="1"/>
       <c r="M36" t="s">
         <v>48</v>
       </c>
@@ -6198,17 +6198,17 @@
         <f>AV37</f>
       </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="2" t="str">
+      <c r="G37" s="1" t="str">
         <f>AV37/AU37-1</f>
       </c>
-      <c r="H37" s="2" t="str">
+      <c r="H37" s="1" t="str">
         <f>AV37/AS37-1</f>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2" t="str">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1" t="str">
         <f>AV37/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K37" s="2"/>
+      <c r="K37" s="1"/>
       <c r="M37" t="s">
         <v>48</v>
       </c>
@@ -6316,17 +6316,17 @@
         <f>AV38</f>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="2" t="str">
+      <c r="G38" s="1" t="str">
         <f>AV38/AU38-1</f>
       </c>
-      <c r="H38" s="2" t="str">
+      <c r="H38" s="1" t="str">
         <f>AV38/AS38-1</f>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2" t="str">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="str">
         <f>AV38/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K38" s="2"/>
+      <c r="K38" s="1"/>
       <c r="M38" t="s">
         <v>48</v>
       </c>
@@ -6432,17 +6432,17 @@
         <f>AV39</f>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="2" t="str">
+      <c r="G39" s="1" t="str">
         <f>AV39/AU39-1</f>
       </c>
-      <c r="H39" s="2" t="str">
+      <c r="H39" s="1" t="str">
         <f>AV39/AS39-1</f>
       </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2" t="str">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1" t="str">
         <f>AV39/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K39" s="2"/>
+      <c r="K39" s="1"/>
       <c r="M39" t="s">
         <v>48</v>
       </c>
@@ -6508,17 +6508,17 @@
         <f>AV40</f>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="2" t="str">
+      <c r="G40" s="1" t="str">
         <f>AV40/AU40-1</f>
       </c>
-      <c r="H40" s="2" t="str">
+      <c r="H40" s="1" t="str">
         <f>AV40/AS40-1</f>
       </c>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2" t="str">
+      <c r="I40" s="1"/>
+      <c r="J40" s="1" t="str">
         <f>AV40/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K40" s="2"/>
+      <c r="K40" s="1"/>
       <c r="M40" t="s">
         <v>48</v>
       </c>
@@ -6622,17 +6622,17 @@
         <f>AV41</f>
       </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="2" t="str">
+      <c r="G41" s="1" t="str">
         <f>AV41/AU41-1</f>
       </c>
-      <c r="H41" s="2" t="str">
+      <c r="H41" s="1" t="str">
         <f>AV41/AS41-1</f>
       </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2" t="str">
+      <c r="I41" s="1"/>
+      <c r="J41" s="1" t="str">
         <f>AV41/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K41" s="2"/>
+      <c r="K41" s="1"/>
       <c r="M41" t="s">
         <v>48</v>
       </c>
@@ -6740,17 +6740,17 @@
         <f>AV42</f>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="2" t="str">
+      <c r="G42" s="1" t="str">
         <f>AV42/AU42-1</f>
       </c>
-      <c r="H42" s="2" t="str">
+      <c r="H42" s="1" t="str">
         <f>AV42/AS42-1</f>
       </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2" t="str">
+      <c r="I42" s="1"/>
+      <c r="J42" s="1" t="str">
         <f>AV42/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K42" s="2"/>
+      <c r="K42" s="1"/>
       <c r="M42" t="s">
         <v>49</v>
       </c>
@@ -6858,17 +6858,17 @@
         <f>AV43</f>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="2" t="str">
+      <c r="G43" s="1" t="str">
         <f>AV43/AU43-1</f>
       </c>
-      <c r="H43" s="2" t="str">
+      <c r="H43" s="1" t="str">
         <f>AV43/AS43-1</f>
       </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2" t="str">
+      <c r="I43" s="1"/>
+      <c r="J43" s="1" t="str">
         <f>AV43/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K43" s="2"/>
+      <c r="K43" s="1"/>
       <c r="M43" t="s">
         <v>49</v>
       </c>
@@ -6976,17 +6976,17 @@
         <f>AV44</f>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44" s="2" t="str">
+      <c r="G44" s="1" t="str">
         <f>AV44/AU44-1</f>
       </c>
-      <c r="H44" s="2" t="str">
+      <c r="H44" s="1" t="str">
         <f>AV44/AS44-1</f>
       </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2" t="str">
+      <c r="I44" s="1"/>
+      <c r="J44" s="1" t="str">
         <f>AV44/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K44" s="2"/>
+      <c r="K44" s="1"/>
       <c r="M44" t="s">
         <v>49</v>
       </c>
@@ -7094,17 +7094,17 @@
         <f>AV45</f>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="2" t="str">
+      <c r="G45" s="1" t="str">
         <f>AV45/AU45-1</f>
       </c>
-      <c r="H45" s="2" t="str">
+      <c r="H45" s="1" t="str">
         <f>AV45/AS45-1</f>
       </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2" t="str">
+      <c r="I45" s="1"/>
+      <c r="J45" s="1" t="str">
         <f>AV45/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K45" s="2"/>
+      <c r="K45" s="1"/>
       <c r="M45" t="s">
         <v>49</v>
       </c>
@@ -7212,17 +7212,17 @@
         <f>AV46</f>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="2" t="str">
+      <c r="G46" s="1" t="str">
         <f>AV46/AU46-1</f>
       </c>
-      <c r="H46" s="2" t="str">
+      <c r="H46" s="1" t="str">
         <f>AV46/AS46-1</f>
       </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2" t="str">
+      <c r="I46" s="1"/>
+      <c r="J46" s="1" t="str">
         <f>AV46/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K46" s="2"/>
+      <c r="K46" s="1"/>
       <c r="M46" t="s">
         <v>49</v>
       </c>
@@ -7330,17 +7330,17 @@
         <f>AV47</f>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="2" t="str">
+      <c r="G47" s="1" t="str">
         <f>AV47/AU47-1</f>
       </c>
-      <c r="H47" s="2" t="str">
+      <c r="H47" s="1" t="str">
         <f>AV47/AS47-1</f>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2" t="str">
+      <c r="I47" s="1"/>
+      <c r="J47" s="1" t="str">
         <f>AV47/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K47" s="2"/>
+      <c r="K47" s="1"/>
       <c r="M47" t="s">
         <v>49</v>
       </c>
@@ -7448,17 +7448,17 @@
         <f>AV48</f>
       </c>
       <c r="F48" s="3"/>
-      <c r="G48" s="2" t="str">
+      <c r="G48" s="1" t="str">
         <f>AV48/AU48-1</f>
       </c>
-      <c r="H48" s="2" t="str">
+      <c r="H48" s="1" t="str">
         <f>AV48/AS48-1</f>
       </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2" t="str">
+      <c r="I48" s="1"/>
+      <c r="J48" s="1" t="str">
         <f>AV48/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K48" s="2"/>
+      <c r="K48" s="1"/>
       <c r="M48"/>
       <c r="N48" t="s">
         <v>36</v>
@@ -7546,17 +7546,17 @@
         <f>AV49</f>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="2" t="str">
+      <c r="G49" s="1" t="str">
         <f>AV49/AU49-1</f>
       </c>
-      <c r="H49" s="2" t="str">
+      <c r="H49" s="1" t="str">
         <f>AV49/AS49-1</f>
       </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2" t="str">
+      <c r="I49" s="1"/>
+      <c r="J49" s="1" t="str">
         <f>AV49/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K49" s="2"/>
+      <c r="K49" s="1"/>
       <c r="M49"/>
       <c r="N49" t="s">
         <v>37</v>
@@ -7666,17 +7666,17 @@
         <f>AV50</f>
       </c>
       <c r="F50" s="3"/>
-      <c r="G50" s="2" t="str">
+      <c r="G50" s="1" t="str">
         <f>AV50/AU50-1</f>
       </c>
-      <c r="H50" s="2" t="str">
+      <c r="H50" s="1" t="str">
         <f>AV50/AS50-1</f>
       </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2" t="str">
+      <c r="I50" s="1"/>
+      <c r="J50" s="1" t="str">
         <f>AV50/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K50" s="2"/>
+      <c r="K50" s="1"/>
       <c r="M50"/>
       <c r="N50" t="s">
         <v>38</v>
@@ -7766,17 +7766,17 @@
         <f>AV51</f>
       </c>
       <c r="F51" s="3"/>
-      <c r="G51" s="2" t="str">
+      <c r="G51" s="1" t="str">
         <f>AV51/AU51-1</f>
       </c>
-      <c r="H51" s="2" t="str">
+      <c r="H51" s="1" t="str">
         <f>AV51/AS51-1</f>
       </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2" t="str">
+      <c r="I51" s="1"/>
+      <c r="J51" s="1" t="str">
         <f>AV51/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K51" s="2"/>
+      <c r="K51" s="1"/>
       <c r="M51"/>
       <c r="N51" t="s">
         <v>42</v>
@@ -7846,17 +7846,17 @@
         <f>AV52</f>
       </c>
       <c r="F52" s="3"/>
-      <c r="G52" s="2" t="str">
+      <c r="G52" s="1" t="str">
         <f>AV52/AU52-1</f>
       </c>
-      <c r="H52" s="2" t="str">
+      <c r="H52" s="1" t="str">
         <f>AV52/AS52-1</f>
       </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2" t="str">
+      <c r="I52" s="1"/>
+      <c r="J52" s="1" t="str">
         <f>AV52/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K52" s="2"/>
+      <c r="K52" s="1"/>
       <c r="M52"/>
       <c r="N52" t="s">
         <v>41</v>
@@ -7982,17 +7982,17 @@
         <f>AV53</f>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="2" t="str">
+      <c r="G53" s="1" t="str">
         <f>AV53/AU53-1</f>
       </c>
-      <c r="H53" s="2" t="str">
+      <c r="H53" s="1" t="str">
         <f>AV53/AS53-1</f>
       </c>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2" t="str">
+      <c r="I53" s="1"/>
+      <c r="J53" s="1" t="str">
         <f>AV53/Sum(AV$29:AV$53)</f>
       </c>
-      <c r="K53" s="2"/>
+      <c r="K53" s="1"/>
       <c r="M53"/>
       <c r="N53" t="s">
         <v>39</v>
@@ -8088,17 +8088,17 @@
         <f>AV54</f>
       </c>
       <c r="F54" s="3"/>
-      <c r="G54" s="2" t="str">
+      <c r="G54" s="1" t="str">
         <f>AV54/AU54-1</f>
       </c>
-      <c r="H54" s="2" t="str">
+      <c r="H54" s="1" t="str">
         <f>AV54/AS54-1</f>
       </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2" t="str">
+      <c r="I54" s="1"/>
+      <c r="J54" s="1" t="str">
         <f>Sum(J$29:J$53)</f>
       </c>
-      <c r="K54" s="2"/>
+      <c r="K54" s="1"/>
       <c r="M54" t="s">
         <v>43</v>
       </c>

</xml_diff>